<commit_message>
update dataElements add/update api
</commit_message>
<xml_diff>
--- a/sample-format/dataElementsPost.xlsx
+++ b/sample-format/dataElementsPost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mithilesh Thakur\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744EBF52-0006-4F05-BA2C-023F30FBA957}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6068AD04-F4CC-4631-A338-35CD89F052BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="415">
   <si>
     <t>name</t>
   </si>
@@ -1270,6 +1270,12 @@
   </si>
   <si>
     <t>kguWskGWWQ3</t>
+  </si>
+  <si>
+    <t>zeroIsSignificant</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -1338,7 +1344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1348,6 +1354,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1663,10 +1672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
-  <dimension ref="A1:I416"/>
+  <dimension ref="A1:J416"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1678,9 +1687,10 @@
     <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1708,8 +1718,11 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J1" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>280</v>
       </c>
@@ -1735,8 +1748,11 @@
       <c r="I2" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J2" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>281</v>
       </c>
@@ -1761,8 +1777,11 @@
       <c r="I3" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J3" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>282</v>
       </c>
@@ -1787,8 +1806,11 @@
       <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J4" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>283</v>
       </c>
@@ -1813,8 +1835,11 @@
       <c r="I5" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J5" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>284</v>
       </c>
@@ -1839,8 +1864,11 @@
       <c r="I6" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J6" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>285</v>
       </c>
@@ -1865,8 +1893,11 @@
       <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J7" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>286</v>
       </c>
@@ -1891,8 +1922,11 @@
       <c r="I8" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J8" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>287</v>
       </c>
@@ -1917,8 +1951,11 @@
       <c r="I9" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J9" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>288</v>
       </c>
@@ -1943,8 +1980,11 @@
       <c r="I10" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J10" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>289</v>
       </c>
@@ -1969,8 +2009,11 @@
       <c r="I11" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J11" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>290</v>
       </c>
@@ -1995,8 +2038,11 @@
       <c r="I12" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J12" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>291</v>
       </c>
@@ -2021,8 +2067,11 @@
       <c r="I13" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J13" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>292</v>
       </c>
@@ -2047,8 +2096,11 @@
       <c r="I14" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J14" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>293</v>
       </c>
@@ -2073,8 +2125,11 @@
       <c r="I15" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J15" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>294</v>
       </c>
@@ -2099,8 +2154,11 @@
       <c r="I16" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J16" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>295</v>
       </c>
@@ -2125,8 +2183,11 @@
       <c r="I17" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J17" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>296</v>
       </c>
@@ -2151,8 +2212,11 @@
       <c r="I18" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J18" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>297</v>
       </c>
@@ -2177,8 +2241,11 @@
       <c r="I19" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J19" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>298</v>
       </c>
@@ -2203,8 +2270,11 @@
       <c r="I20" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J20" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>299</v>
       </c>
@@ -2229,8 +2299,11 @@
       <c r="I21" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J21" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>300</v>
       </c>
@@ -2255,8 +2328,11 @@
       <c r="I22" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J22" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>301</v>
       </c>
@@ -2281,8 +2357,11 @@
       <c r="I23" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J23" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>302</v>
       </c>
@@ -2307,8 +2386,11 @@
       <c r="I24" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J24" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>303</v>
       </c>
@@ -2333,8 +2415,11 @@
       <c r="I25" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J25" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>304</v>
       </c>
@@ -2359,8 +2444,11 @@
       <c r="I26" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J26" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>305</v>
       </c>
@@ -2385,8 +2473,11 @@
       <c r="I27" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J27" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>306</v>
       </c>
@@ -2411,8 +2502,11 @@
       <c r="I28" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J28" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>307</v>
       </c>
@@ -2437,8 +2531,11 @@
       <c r="I29" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J29" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>308</v>
       </c>
@@ -2463,8 +2560,11 @@
       <c r="I30" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J30" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>309</v>
       </c>
@@ -2489,8 +2589,11 @@
       <c r="I31" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J31" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>310</v>
       </c>
@@ -2515,8 +2618,11 @@
       <c r="I32" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J32" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>311</v>
       </c>
@@ -2541,8 +2647,11 @@
       <c r="I33" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J33" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>312</v>
       </c>
@@ -2567,8 +2676,11 @@
       <c r="I34" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J34" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>313</v>
       </c>
@@ -2593,8 +2705,11 @@
       <c r="I35" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J35" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>314</v>
       </c>
@@ -2619,8 +2734,11 @@
       <c r="I36" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J36" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>315</v>
       </c>
@@ -2645,8 +2763,11 @@
       <c r="I37" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J37" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>316</v>
       </c>
@@ -2671,8 +2792,11 @@
       <c r="I38" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J38" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>317</v>
       </c>
@@ -2697,8 +2821,11 @@
       <c r="I39" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J39" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>318</v>
       </c>
@@ -2723,8 +2850,11 @@
       <c r="I40" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J40" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>319</v>
       </c>
@@ -2749,8 +2879,11 @@
       <c r="I41" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J41" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>320</v>
       </c>
@@ -2775,8 +2908,11 @@
       <c r="I42" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J42" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>321</v>
       </c>
@@ -2801,8 +2937,11 @@
       <c r="I43" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J43" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>322</v>
       </c>
@@ -2827,8 +2966,11 @@
       <c r="I44" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J44" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>323</v>
       </c>
@@ -2853,8 +2995,11 @@
       <c r="I45" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J45" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>324</v>
       </c>
@@ -2879,8 +3024,11 @@
       <c r="I46" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J46" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>325</v>
       </c>
@@ -2905,8 +3053,11 @@
       <c r="I47" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J47" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>326</v>
       </c>
@@ -2931,8 +3082,11 @@
       <c r="I48" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J48" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>327</v>
       </c>
@@ -2957,8 +3111,11 @@
       <c r="I49" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J49" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>328</v>
       </c>
@@ -2983,8 +3140,11 @@
       <c r="I50" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J50" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>329</v>
       </c>
@@ -3009,8 +3169,11 @@
       <c r="I51" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J51" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>330</v>
       </c>
@@ -3035,8 +3198,11 @@
       <c r="I52" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J52" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>331</v>
       </c>
@@ -3061,8 +3227,11 @@
       <c r="I53" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J53" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>332</v>
       </c>
@@ -3087,8 +3256,11 @@
       <c r="I54" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J54" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>333</v>
       </c>
@@ -3113,8 +3285,11 @@
       <c r="I55" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J55" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>334</v>
       </c>
@@ -3139,8 +3314,11 @@
       <c r="I56" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J56" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>335</v>
       </c>
@@ -3165,8 +3343,11 @@
       <c r="I57" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J57" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>336</v>
       </c>
@@ -3191,8 +3372,11 @@
       <c r="I58" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J58" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>337</v>
       </c>
@@ -3217,8 +3401,11 @@
       <c r="I59" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J59" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>338</v>
       </c>
@@ -3243,8 +3430,11 @@
       <c r="I60" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J60" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>339</v>
       </c>
@@ -3269,8 +3459,11 @@
       <c r="I61" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J61" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>340</v>
       </c>
@@ -3295,8 +3488,11 @@
       <c r="I62" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J62" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>341</v>
       </c>
@@ -3321,8 +3517,11 @@
       <c r="I63" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J63" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>342</v>
       </c>
@@ -3347,8 +3546,11 @@
       <c r="I64" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J64" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>343</v>
       </c>
@@ -3373,8 +3575,11 @@
       <c r="I65" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J65" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>344</v>
       </c>
@@ -3399,8 +3604,11 @@
       <c r="I66" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J66" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>345</v>
       </c>
@@ -3425,8 +3633,11 @@
       <c r="I67" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J67" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>346</v>
       </c>
@@ -3451,8 +3662,11 @@
       <c r="I68" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J68" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>347</v>
       </c>
@@ -3477,8 +3691,11 @@
       <c r="I69" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J69" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>348</v>
       </c>
@@ -3503,8 +3720,11 @@
       <c r="I70" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J70" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>349</v>
       </c>
@@ -3529,8 +3749,11 @@
       <c r="I71" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J71" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>350</v>
       </c>
@@ -3555,8 +3778,11 @@
       <c r="I72" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J72" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>351</v>
       </c>
@@ -3581,8 +3807,11 @@
       <c r="I73" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J73" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>352</v>
       </c>
@@ -3607,8 +3836,11 @@
       <c r="I74" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J74" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>353</v>
       </c>
@@ -3633,8 +3865,11 @@
       <c r="I75" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J75" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>354</v>
       </c>
@@ -3659,8 +3894,11 @@
       <c r="I76" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J76" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>355</v>
       </c>
@@ -3685,8 +3923,11 @@
       <c r="I77" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J77" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>356</v>
       </c>
@@ -3711,8 +3952,11 @@
       <c r="I78" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J78" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>357</v>
       </c>
@@ -3737,8 +3981,11 @@
       <c r="I79" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J79" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>358</v>
       </c>
@@ -3763,8 +4010,11 @@
       <c r="I80" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J80" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>359</v>
       </c>
@@ -3789,8 +4039,11 @@
       <c r="I81" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J81" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>360</v>
       </c>
@@ -3815,8 +4068,11 @@
       <c r="I82" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J82" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>361</v>
       </c>
@@ -3841,8 +4097,11 @@
       <c r="I83" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J83" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>362</v>
       </c>
@@ -3867,8 +4126,11 @@
       <c r="I84" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J84" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>363</v>
       </c>
@@ -3893,8 +4155,11 @@
       <c r="I85" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J85" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>364</v>
       </c>
@@ -3919,8 +4184,11 @@
       <c r="I86" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J86" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>365</v>
       </c>
@@ -3945,8 +4213,11 @@
       <c r="I87" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J87" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>366</v>
       </c>
@@ -3971,8 +4242,11 @@
       <c r="I88" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J88" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>367</v>
       </c>
@@ -3997,8 +4271,11 @@
       <c r="I89" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J89" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>368</v>
       </c>
@@ -4023,8 +4300,11 @@
       <c r="I90" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J90" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>369</v>
       </c>
@@ -4049,8 +4329,11 @@
       <c r="I91" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J91" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>370</v>
       </c>
@@ -4075,8 +4358,11 @@
       <c r="I92" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J92" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="93" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>371</v>
       </c>
@@ -4101,8 +4387,11 @@
       <c r="I93" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J93" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>372</v>
       </c>
@@ -4127,8 +4416,11 @@
       <c r="I94" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J94" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="95" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>373</v>
       </c>
@@ -4153,8 +4445,11 @@
       <c r="I95" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J95" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="96" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>374</v>
       </c>
@@ -4179,8 +4474,11 @@
       <c r="I96" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J96" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>375</v>
       </c>
@@ -4205,8 +4503,11 @@
       <c r="I97" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J97" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>376</v>
       </c>
@@ -4231,8 +4532,11 @@
       <c r="I98" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J98" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>377</v>
       </c>
@@ -4257,8 +4561,11 @@
       <c r="I99" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J99" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>378</v>
       </c>
@@ -4283,8 +4590,11 @@
       <c r="I100" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J100" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="101" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>379</v>
       </c>
@@ -4309,8 +4619,11 @@
       <c r="I101" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J101" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>380</v>
       </c>
@@ -4335,8 +4648,11 @@
       <c r="I102" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J102" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>381</v>
       </c>
@@ -4361,8 +4677,11 @@
       <c r="I103" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J103" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>382</v>
       </c>
@@ -4387,8 +4706,11 @@
       <c r="I104" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J104" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>383</v>
       </c>
@@ -4413,8 +4735,11 @@
       <c r="I105" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J105" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>384</v>
       </c>
@@ -4439,8 +4764,11 @@
       <c r="I106" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J106" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>385</v>
       </c>
@@ -4465,8 +4793,11 @@
       <c r="I107" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J107" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>386</v>
       </c>
@@ -4491,8 +4822,11 @@
       <c r="I108" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J108" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="109" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>387</v>
       </c>
@@ -4517,8 +4851,11 @@
       <c r="I109" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J109" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>388</v>
       </c>
@@ -4543,8 +4880,11 @@
       <c r="I110" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J110" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>389</v>
       </c>
@@ -4569,8 +4909,11 @@
       <c r="I111" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J111" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>390</v>
       </c>
@@ -4595,8 +4938,11 @@
       <c r="I112" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J112" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>391</v>
       </c>
@@ -4621,8 +4967,11 @@
       <c r="I113" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J113" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>392</v>
       </c>
@@ -4647,8 +4996,11 @@
       <c r="I114" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J114" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>393</v>
       </c>
@@ -4673,8 +5025,11 @@
       <c r="I115" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J115" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>394</v>
       </c>
@@ -4699,8 +5054,11 @@
       <c r="I116" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J116" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>395</v>
       </c>
@@ -4725,8 +5083,11 @@
       <c r="I117" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J117" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>396</v>
       </c>
@@ -4751,8 +5112,11 @@
       <c r="I118" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J118" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>397</v>
       </c>
@@ -4777,8 +5141,11 @@
       <c r="I119" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J119" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>398</v>
       </c>
@@ -4803,8 +5170,11 @@
       <c r="I120" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J120" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>399</v>
       </c>
@@ -4829,8 +5199,11 @@
       <c r="I121" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J121" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>400</v>
       </c>
@@ -4855,8 +5228,11 @@
       <c r="I122" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J122" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>401</v>
       </c>
@@ -4881,8 +5257,11 @@
       <c r="I123" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J123" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>402</v>
       </c>
@@ -4907,8 +5286,11 @@
       <c r="I124" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J124" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>403</v>
       </c>
@@ -4933,8 +5315,11 @@
       <c r="I125" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J125" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>404</v>
       </c>
@@ -4959,8 +5344,11 @@
       <c r="I126" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J126" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="127" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -4985,8 +5373,11 @@
       <c r="I127" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J127" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>406</v>
       </c>
@@ -5011,8 +5402,11 @@
       <c r="I128" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J128" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>407</v>
       </c>
@@ -5037,8 +5431,11 @@
       <c r="I129" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J129" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>408</v>
       </c>
@@ -5063,8 +5460,11 @@
       <c r="I130" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J130" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>409</v>
       </c>
@@ -5089,8 +5489,11 @@
       <c r="I131" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J131" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="132" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>410</v>
       </c>
@@ -5115,8 +5518,11 @@
       <c r="I132" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J132" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>411</v>
       </c>
@@ -5141,8 +5547,11 @@
       <c r="I133" s="5" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J133" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>412</v>
       </c>
@@ -5167,53 +5576,56 @@
       <c r="I134" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+      <c r="J134" s="8" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -6585,15 +6997,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010064994C001712374395B345EB88ED991F" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8c1a62579524e26006c6d5335831b55c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9770305-a86c-4dd4-a8e3-5283c3e6bf99" xmlns:ns3="3f48127a-ff27-4c8f-88c3-e54b29f41588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="658091719f3253a39288b5ed2add5a7b" ns2:_="" ns3:_="">
     <xsd:import namespace="f9770305-a86c-4dd4-a8e3-5283c3e6bf99"/>
@@ -6790,6 +7193,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6797,14 +7209,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E76993AC-6818-4630-B1D6-F654BE5E03B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6823,6 +7227,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18A4371F-7DC5-4CF4-A869-E47776CCD6EB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ACBAC26C-ABD4-4796-8551-545E34A88729}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
update dataElement post sheet format
</commit_message>
<xml_diff>
--- a/sample-format/dataElementsPost.xlsx
+++ b/sample-format/dataElementsPost.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitHub_source_code\excel_to_Json_Converter_angularJS\sample-format\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6068AD04-F4CC-4631-A338-35CD89F052BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E5F6B1B-65B3-4F1F-8011-30B51C197146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1207" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1074" uniqueCount="414">
   <si>
     <t>name</t>
   </si>
@@ -1273,9 +1273,6 @@
   </si>
   <si>
     <t>zeroIsSignificant</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
 </sst>
 </file>
@@ -1674,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E6B5FAB-DF4A-42DC-8643-A674828EC12D}">
   <dimension ref="A1:J416"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1687,7 +1684,7 @@
     <col min="6" max="6" width="13.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.36328125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.90625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="13.5" x14ac:dyDescent="0.35">
@@ -1718,7 +1715,7 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="8" t="s">
         <v>413</v>
       </c>
     </row>
@@ -1748,8 +1745,8 @@
       <c r="I2" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J2" s="8" t="s">
-        <v>414</v>
+      <c r="J2" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
@@ -1777,8 +1774,8 @@
       <c r="I3" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J3" s="8" t="s">
-        <v>414</v>
+      <c r="J3" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
@@ -1806,8 +1803,8 @@
       <c r="I4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J4" s="8" t="s">
-        <v>414</v>
+      <c r="J4" s="8" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
@@ -1835,9 +1832,6 @@
       <c r="I5" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J5" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -1864,9 +1858,6 @@
       <c r="I6" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J6" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="7" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -1893,9 +1884,6 @@
       <c r="I7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J7" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="8" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -1922,9 +1910,6 @@
       <c r="I8" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J8" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="9" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -1951,9 +1936,6 @@
       <c r="I9" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J9" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="10" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -1980,9 +1962,6 @@
       <c r="I10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J10" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="11" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -2009,9 +1988,6 @@
       <c r="I11" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J11" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="12" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -2038,9 +2014,6 @@
       <c r="I12" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J12" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="13" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -2067,9 +2040,6 @@
       <c r="I13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="14" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2096,9 +2066,6 @@
       <c r="I14" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J14" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="15" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -2125,9 +2092,6 @@
       <c r="I15" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J15" s="8" t="s">
-        <v>414</v>
-      </c>
     </row>
     <row r="16" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -2154,11 +2118,8 @@
       <c r="I16" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>295</v>
       </c>
@@ -2183,11 +2144,8 @@
       <c r="I17" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J17" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>296</v>
       </c>
@@ -2212,11 +2170,8 @@
       <c r="I18" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J18" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>297</v>
       </c>
@@ -2241,11 +2196,8 @@
       <c r="I19" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>298</v>
       </c>
@@ -2270,11 +2222,8 @@
       <c r="I20" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J20" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>299</v>
       </c>
@@ -2299,11 +2248,8 @@
       <c r="I21" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J21" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>300</v>
       </c>
@@ -2328,11 +2274,8 @@
       <c r="I22" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J22" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>301</v>
       </c>
@@ -2357,11 +2300,8 @@
       <c r="I23" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J23" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>302</v>
       </c>
@@ -2386,11 +2326,8 @@
       <c r="I24" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J24" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>303</v>
       </c>
@@ -2415,11 +2352,8 @@
       <c r="I25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J25" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>304</v>
       </c>
@@ -2444,11 +2378,8 @@
       <c r="I26" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J26" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>305</v>
       </c>
@@ -2473,11 +2404,8 @@
       <c r="I27" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>306</v>
       </c>
@@ -2502,11 +2430,8 @@
       <c r="I28" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J28" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
         <v>307</v>
       </c>
@@ -2531,11 +2456,8 @@
       <c r="I29" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J29" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>308</v>
       </c>
@@ -2560,11 +2482,8 @@
       <c r="I30" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J30" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>309</v>
       </c>
@@ -2589,11 +2508,8 @@
       <c r="I31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J31" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>310</v>
       </c>
@@ -2618,11 +2534,8 @@
       <c r="I32" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J32" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
         <v>311</v>
       </c>
@@ -2647,11 +2560,8 @@
       <c r="I33" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J33" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>312</v>
       </c>
@@ -2676,11 +2586,8 @@
       <c r="I34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J34" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>313</v>
       </c>
@@ -2705,11 +2612,8 @@
       <c r="I35" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J35" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
         <v>314</v>
       </c>
@@ -2734,11 +2638,8 @@
       <c r="I36" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J36" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>315</v>
       </c>
@@ -2763,11 +2664,8 @@
       <c r="I37" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J37" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>316</v>
       </c>
@@ -2792,11 +2690,8 @@
       <c r="I38" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J38" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>317</v>
       </c>
@@ -2821,11 +2716,8 @@
       <c r="I39" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J39" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>318</v>
       </c>
@@ -2850,11 +2742,8 @@
       <c r="I40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J40" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
         <v>319</v>
       </c>
@@ -2879,11 +2768,8 @@
       <c r="I41" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J41" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>320</v>
       </c>
@@ -2908,11 +2794,8 @@
       <c r="I42" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J42" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>321</v>
       </c>
@@ -2937,11 +2820,8 @@
       <c r="I43" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J43" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>322</v>
       </c>
@@ -2966,11 +2846,8 @@
       <c r="I44" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J44" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>323</v>
       </c>
@@ -2995,11 +2872,8 @@
       <c r="I45" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J45" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
         <v>324</v>
       </c>
@@ -3024,11 +2898,8 @@
       <c r="I46" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J46" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
         <v>325</v>
       </c>
@@ -3053,11 +2924,8 @@
       <c r="I47" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J47" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
         <v>326</v>
       </c>
@@ -3082,11 +2950,8 @@
       <c r="I48" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J48" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
         <v>327</v>
       </c>
@@ -3111,11 +2976,8 @@
       <c r="I49" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J49" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
         <v>328</v>
       </c>
@@ -3140,11 +3002,8 @@
       <c r="I50" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J50" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
         <v>329</v>
       </c>
@@ -3169,11 +3028,8 @@
       <c r="I51" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J51" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
         <v>330</v>
       </c>
@@ -3198,11 +3054,8 @@
       <c r="I52" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J52" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
         <v>331</v>
       </c>
@@ -3227,11 +3080,8 @@
       <c r="I53" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J53" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
         <v>332</v>
       </c>
@@ -3256,11 +3106,8 @@
       <c r="I54" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J54" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
         <v>333</v>
       </c>
@@ -3285,11 +3132,8 @@
       <c r="I55" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J55" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
         <v>334</v>
       </c>
@@ -3314,11 +3158,8 @@
       <c r="I56" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J56" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
         <v>335</v>
       </c>
@@ -3343,11 +3184,8 @@
       <c r="I57" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J57" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
         <v>336</v>
       </c>
@@ -3372,11 +3210,8 @@
       <c r="I58" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J58" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
         <v>337</v>
       </c>
@@ -3401,11 +3236,8 @@
       <c r="I59" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J59" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
         <v>338</v>
       </c>
@@ -3430,11 +3262,8 @@
       <c r="I60" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J60" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
         <v>339</v>
       </c>
@@ -3459,11 +3288,8 @@
       <c r="I61" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J61" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
         <v>340</v>
       </c>
@@ -3488,11 +3314,8 @@
       <c r="I62" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J62" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
         <v>341</v>
       </c>
@@ -3517,11 +3340,8 @@
       <c r="I63" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J63" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
         <v>342</v>
       </c>
@@ -3546,11 +3366,8 @@
       <c r="I64" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J64" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
         <v>343</v>
       </c>
@@ -3575,11 +3392,8 @@
       <c r="I65" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J65" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
         <v>344</v>
       </c>
@@ -3604,11 +3418,8 @@
       <c r="I66" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J66" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
         <v>345</v>
       </c>
@@ -3633,11 +3444,8 @@
       <c r="I67" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J67" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
         <v>346</v>
       </c>
@@ -3662,11 +3470,8 @@
       <c r="I68" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J68" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
         <v>347</v>
       </c>
@@ -3691,11 +3496,8 @@
       <c r="I69" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J69" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
         <v>348</v>
       </c>
@@ -3720,11 +3522,8 @@
       <c r="I70" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J70" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
         <v>349</v>
       </c>
@@ -3749,11 +3548,8 @@
       <c r="I71" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J71" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
         <v>350</v>
       </c>
@@ -3778,11 +3574,8 @@
       <c r="I72" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J72" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
         <v>351</v>
       </c>
@@ -3807,11 +3600,8 @@
       <c r="I73" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J73" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
         <v>352</v>
       </c>
@@ -3836,11 +3626,8 @@
       <c r="I74" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J74" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
         <v>353</v>
       </c>
@@ -3865,11 +3652,8 @@
       <c r="I75" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J75" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
         <v>354</v>
       </c>
@@ -3894,11 +3678,8 @@
       <c r="I76" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J76" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
         <v>355</v>
       </c>
@@ -3923,11 +3704,8 @@
       <c r="I77" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J77" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
         <v>356</v>
       </c>
@@ -3952,11 +3730,8 @@
       <c r="I78" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J78" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
         <v>357</v>
       </c>
@@ -3981,11 +3756,8 @@
       <c r="I79" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J79" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
         <v>358</v>
       </c>
@@ -4010,11 +3782,8 @@
       <c r="I80" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J80" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
         <v>359</v>
       </c>
@@ -4039,11 +3808,8 @@
       <c r="I81" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J81" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="82" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
         <v>360</v>
       </c>
@@ -4068,11 +3834,8 @@
       <c r="I82" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J82" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="83" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
         <v>361</v>
       </c>
@@ -4097,11 +3860,8 @@
       <c r="I83" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J83" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
         <v>362</v>
       </c>
@@ -4126,11 +3886,8 @@
       <c r="I84" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J84" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="85" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
         <v>363</v>
       </c>
@@ -4155,11 +3912,8 @@
       <c r="I85" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J85" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="86" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
         <v>364</v>
       </c>
@@ -4184,11 +3938,8 @@
       <c r="I86" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J86" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
         <v>365</v>
       </c>
@@ -4213,11 +3964,8 @@
       <c r="I87" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J87" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="88" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
         <v>366</v>
       </c>
@@ -4242,11 +3990,8 @@
       <c r="I88" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J88" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="89" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
         <v>367</v>
       </c>
@@ -4271,11 +4016,8 @@
       <c r="I89" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J89" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="90" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
         <v>368</v>
       </c>
@@ -4300,11 +4042,8 @@
       <c r="I90" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J90" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="91" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="91" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
         <v>369</v>
       </c>
@@ -4329,11 +4068,8 @@
       <c r="I91" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J91" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="92" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="92" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
         <v>370</v>
       </c>
@@ -4358,11 +4094,8 @@
       <c r="I92" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J92" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="93" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="93" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
         <v>371</v>
       </c>
@@ -4387,11 +4120,8 @@
       <c r="I93" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J93" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="94" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="94" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
         <v>372</v>
       </c>
@@ -4416,11 +4146,8 @@
       <c r="I94" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J94" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="95" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="95" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
         <v>373</v>
       </c>
@@ -4445,11 +4172,8 @@
       <c r="I95" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J95" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="96" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="96" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
         <v>374</v>
       </c>
@@ -4474,11 +4198,8 @@
       <c r="I96" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J96" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="97" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
         <v>375</v>
       </c>
@@ -4503,11 +4224,8 @@
       <c r="I97" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J97" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="98" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
         <v>376</v>
       </c>
@@ -4532,11 +4250,8 @@
       <c r="I98" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J98" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="99" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
         <v>377</v>
       </c>
@@ -4561,11 +4276,8 @@
       <c r="I99" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J99" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="100" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="100" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
         <v>378</v>
       </c>
@@ -4590,11 +4302,8 @@
       <c r="I100" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J100" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="101" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="101" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A101" s="7" t="s">
         <v>379</v>
       </c>
@@ -4619,11 +4328,8 @@
       <c r="I101" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J101" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="102" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A102" s="7" t="s">
         <v>380</v>
       </c>
@@ -4648,11 +4354,8 @@
       <c r="I102" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J102" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="103" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A103" s="7" t="s">
         <v>381</v>
       </c>
@@ -4677,11 +4380,8 @@
       <c r="I103" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J103" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="104" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A104" s="7" t="s">
         <v>382</v>
       </c>
@@ -4706,11 +4406,8 @@
       <c r="I104" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J104" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A105" s="7" t="s">
         <v>383</v>
       </c>
@@ -4735,11 +4432,8 @@
       <c r="I105" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J105" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="106" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A106" s="7" t="s">
         <v>384</v>
       </c>
@@ -4764,11 +4458,8 @@
       <c r="I106" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J106" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A107" s="7" t="s">
         <v>385</v>
       </c>
@@ -4793,11 +4484,8 @@
       <c r="I107" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J107" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="108" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A108" s="7" t="s">
         <v>386</v>
       </c>
@@ -4822,11 +4510,8 @@
       <c r="I108" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J108" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="109" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A109" s="7" t="s">
         <v>387</v>
       </c>
@@ -4851,11 +4536,8 @@
       <c r="I109" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J109" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="110" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A110" s="7" t="s">
         <v>388</v>
       </c>
@@ -4880,11 +4562,8 @@
       <c r="I110" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J110" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A111" s="7" t="s">
         <v>389</v>
       </c>
@@ -4909,11 +4588,8 @@
       <c r="I111" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J111" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A112" s="7" t="s">
         <v>390</v>
       </c>
@@ -4938,11 +4614,8 @@
       <c r="I112" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J112" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A113" s="7" t="s">
         <v>391</v>
       </c>
@@ -4967,11 +4640,8 @@
       <c r="I113" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J113" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="114" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A114" s="7" t="s">
         <v>392</v>
       </c>
@@ -4996,11 +4666,8 @@
       <c r="I114" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J114" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="115" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A115" s="7" t="s">
         <v>393</v>
       </c>
@@ -5025,11 +4692,8 @@
       <c r="I115" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J115" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="116" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A116" s="7" t="s">
         <v>394</v>
       </c>
@@ -5054,11 +4718,8 @@
       <c r="I116" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J116" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="117" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="117" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A117" s="7" t="s">
         <v>395</v>
       </c>
@@ -5083,11 +4744,8 @@
       <c r="I117" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J117" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="118" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="118" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A118" s="7" t="s">
         <v>396</v>
       </c>
@@ -5112,11 +4770,8 @@
       <c r="I118" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J118" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="119" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A119" s="7" t="s">
         <v>397</v>
       </c>
@@ -5141,11 +4796,8 @@
       <c r="I119" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J119" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="120" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A120" s="7" t="s">
         <v>398</v>
       </c>
@@ -5170,11 +4822,8 @@
       <c r="I120" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J120" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="121" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A121" s="7" t="s">
         <v>399</v>
       </c>
@@ -5199,11 +4848,8 @@
       <c r="I121" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J121" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="122" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A122" s="7" t="s">
         <v>400</v>
       </c>
@@ -5228,11 +4874,8 @@
       <c r="I122" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J122" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="123" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="123" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A123" s="7" t="s">
         <v>401</v>
       </c>
@@ -5257,11 +4900,8 @@
       <c r="I123" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J123" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="124" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A124" s="7" t="s">
         <v>402</v>
       </c>
@@ -5286,11 +4926,8 @@
       <c r="I124" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J124" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="125" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A125" s="7" t="s">
         <v>403</v>
       </c>
@@ -5315,11 +4952,8 @@
       <c r="I125" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J125" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="126" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A126" s="7" t="s">
         <v>404</v>
       </c>
@@ -5344,11 +4978,8 @@
       <c r="I126" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J126" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="127" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="127" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A127" s="7" t="s">
         <v>405</v>
       </c>
@@ -5373,11 +5004,8 @@
       <c r="I127" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J127" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="128" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="128" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A128" s="7" t="s">
         <v>406</v>
       </c>
@@ -5402,11 +5030,8 @@
       <c r="I128" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J128" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="129" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="129" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A129" s="7" t="s">
         <v>407</v>
       </c>
@@ -5431,11 +5056,8 @@
       <c r="I129" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J129" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="130" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A130" s="7" t="s">
         <v>408</v>
       </c>
@@ -5460,11 +5082,8 @@
       <c r="I130" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J130" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="131" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A131" s="7" t="s">
         <v>409</v>
       </c>
@@ -5489,11 +5108,8 @@
       <c r="I131" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J131" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="132" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="132" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A132" s="7" t="s">
         <v>410</v>
       </c>
@@ -5518,11 +5134,8 @@
       <c r="I132" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J132" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="133" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="133" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A133" s="7" t="s">
         <v>411</v>
       </c>
@@ -5547,11 +5160,8 @@
       <c r="I133" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="J133" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="134" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="134" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A134" s="7" t="s">
         <v>412</v>
       </c>
@@ -5576,56 +5186,53 @@
       <c r="I134" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J134" s="8" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="135" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
     </row>
-    <row r="136" spans="1:10" ht="14.5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
     </row>
-    <row r="137" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
     </row>
-    <row r="139" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
     </row>
-    <row r="140" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
     </row>
-    <row r="141" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
     </row>
-    <row r="142" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>

</xml_diff>